<commit_message>
Minor updates and cleaning
</commit_message>
<xml_diff>
--- a/data/results/exp_5/results_12p_01.xlsx
+++ b/data/results/exp_5/results_12p_01.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danim\Documents\GitHub\PIC-PAPER-01\data\results\exp_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DB756586-005C-474F-864A-39F1DD453E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3187E6E7-E0FA-42E8-8604-5A2B25424FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{03902F72-408F-401B-80FB-ADF521EA75D5}"/>
+    <workbookView xWindow="-90" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{03902F72-408F-401B-80FB-ADF521EA75D5}"/>
   </bookViews>
   <sheets>
     <sheet name="results_12p_01" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">results_12p_01!$A$1:$Q$121</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="117">
   <si>
     <t>Test</t>
   </si>
@@ -371,6 +372,9 @@
   </si>
   <si>
     <t>5,3</t>
+  </si>
+  <si>
+    <t>Parameters</t>
   </si>
 </sst>
 </file>
@@ -1240,8 +1244,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R99" sqref="R99"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7677,4 +7681,1297 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3FA5BC-1E21-428E-A6AE-BF90075B13F9}">
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>0.6321</v>
+      </c>
+      <c r="E2">
+        <v>0.56140000000000001</v>
+      </c>
+      <c r="F2">
+        <v>0.6321</v>
+      </c>
+      <c r="G2">
+        <v>0.58489999999999998</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2">
+        <v>2.8454999999999999</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>112</v>
+      </c>
+      <c r="M2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>0.62609999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.61080000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.62609999999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.56440000000000001</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>0.46550000000000002</v>
+      </c>
+      <c r="E4">
+        <v>0.313</v>
+      </c>
+      <c r="F4">
+        <v>0.46550000000000002</v>
+      </c>
+      <c r="G4">
+        <v>0.3574</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4">
+        <v>0.34160000000000001</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>112</v>
+      </c>
+      <c r="M4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>0.66320000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.66290000000000004</v>
+      </c>
+      <c r="F5">
+        <v>0.66320000000000001</v>
+      </c>
+      <c r="G5">
+        <v>0.59089999999999998</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5">
+        <v>397.07130000000001</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>112</v>
+      </c>
+      <c r="M5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>0.37559999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.29509999999999997</v>
+      </c>
+      <c r="F6">
+        <v>0.37559999999999999</v>
+      </c>
+      <c r="G6">
+        <v>0.28510000000000002</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="K6">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>112</v>
+      </c>
+      <c r="M6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>0.65539999999999998</v>
+      </c>
+      <c r="E7">
+        <v>0.5978</v>
+      </c>
+      <c r="F7">
+        <v>0.65539999999999998</v>
+      </c>
+      <c r="G7">
+        <v>0.58609999999999995</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7">
+        <v>1.794</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>112</v>
+      </c>
+      <c r="M7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>0.87739999999999996</v>
+      </c>
+      <c r="E8">
+        <v>0.8458</v>
+      </c>
+      <c r="F8">
+        <v>0.87739999999999996</v>
+      </c>
+      <c r="G8">
+        <v>0.85409999999999997</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>0.73319999999999996</v>
+      </c>
+      <c r="E9">
+        <v>0.62060000000000004</v>
+      </c>
+      <c r="F9">
+        <v>0.73319999999999996</v>
+      </c>
+      <c r="G9">
+        <v>0.65359999999999996</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>112</v>
+      </c>
+      <c r="M9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>0.51119999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0.37130000000000002</v>
+      </c>
+      <c r="F10">
+        <v>0.51119999999999999</v>
+      </c>
+      <c r="G10">
+        <v>0.40949999999999998</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <v>134.94390000000001</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>112</v>
+      </c>
+      <c r="M10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.64090000000000003</v>
+      </c>
+      <c r="F11">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="G11">
+        <v>0.66539999999999999</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="K11">
+        <v>1E-4</v>
+      </c>
+      <c r="L11" t="s">
+        <v>112</v>
+      </c>
+      <c r="M11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>0.75649999999999995</v>
+      </c>
+      <c r="E12">
+        <v>0.67769999999999997</v>
+      </c>
+      <c r="F12">
+        <v>0.75649999999999995</v>
+      </c>
+      <c r="G12">
+        <v>0.70089999999999997</v>
+      </c>
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12">
+        <v>1.3066</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>112</v>
+      </c>
+      <c r="M12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>0.88</v>
+      </c>
+      <c r="E13">
+        <v>0.84040000000000004</v>
+      </c>
+      <c r="F13">
+        <v>0.88</v>
+      </c>
+      <c r="G13">
+        <v>0.85260000000000002</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>112</v>
+      </c>
+      <c r="M13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>0.74780000000000002</v>
+      </c>
+      <c r="E14">
+        <v>0.62019999999999997</v>
+      </c>
+      <c r="F14">
+        <v>0.74780000000000002</v>
+      </c>
+      <c r="G14">
+        <v>0.66349999999999998</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14">
+        <v>0.2873</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>0.58379999999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.72909999999999997</v>
+      </c>
+      <c r="F15">
+        <v>0.58379999999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.50929999999999997</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15">
+        <v>67.366299999999995</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>112</v>
+      </c>
+      <c r="M15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>0.62439999999999996</v>
+      </c>
+      <c r="E16">
+        <v>0.50770000000000004</v>
+      </c>
+      <c r="F16">
+        <v>0.62439999999999996</v>
+      </c>
+      <c r="G16">
+        <v>0.53339999999999999</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16">
+        <v>2.7E-2</v>
+      </c>
+      <c r="K16">
+        <v>1E-4</v>
+      </c>
+      <c r="L16" t="s">
+        <v>112</v>
+      </c>
+      <c r="M16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="E17">
+        <v>0.73150000000000004</v>
+      </c>
+      <c r="F17">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="G17">
+        <v>0.70730000000000004</v>
+      </c>
+      <c r="H17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17">
+        <v>0.92059999999999997</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>112</v>
+      </c>
+      <c r="M17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>0.85750000000000004</v>
+      </c>
+      <c r="E18">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="F18">
+        <v>0.85750000000000004</v>
+      </c>
+      <c r="G18">
+        <v>0.82569999999999999</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>112</v>
+      </c>
+      <c r="M18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="E19">
+        <v>0.4929</v>
+      </c>
+      <c r="F19">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="G19">
+        <v>0.55279999999999996</v>
+      </c>
+      <c r="H19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19">
+        <v>0.41170000000000001</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>112</v>
+      </c>
+      <c r="M19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>0.56910000000000005</v>
+      </c>
+      <c r="E20">
+        <v>0.70840000000000003</v>
+      </c>
+      <c r="F20">
+        <v>0.56910000000000005</v>
+      </c>
+      <c r="G20">
+        <v>0.50290000000000001</v>
+      </c>
+      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20">
+        <v>35.489400000000003</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>112</v>
+      </c>
+      <c r="M20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>0.73829999999999996</v>
+      </c>
+      <c r="E21">
+        <v>0.64319999999999999</v>
+      </c>
+      <c r="F21">
+        <v>0.73829999999999996</v>
+      </c>
+      <c r="G21">
+        <v>0.66990000000000005</v>
+      </c>
+      <c r="H21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21">
+        <v>2.9499999999999998E-2</v>
+      </c>
+      <c r="K21">
+        <v>1E-4</v>
+      </c>
+      <c r="L21" t="s">
+        <v>112</v>
+      </c>
+      <c r="M21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>0.81</v>
+      </c>
+      <c r="E22">
+        <v>0.87670000000000003</v>
+      </c>
+      <c r="F22">
+        <v>0.81</v>
+      </c>
+      <c r="G22">
+        <v>0.78720000000000001</v>
+      </c>
+      <c r="H22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" t="s">
+        <v>50</v>
+      </c>
+      <c r="J22">
+        <v>0.50209999999999999</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>114</v>
+      </c>
+      <c r="M22">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>0.79969999999999997</v>
+      </c>
+      <c r="E23">
+        <v>0.87180000000000002</v>
+      </c>
+      <c r="F23">
+        <v>0.79969999999999997</v>
+      </c>
+      <c r="G23">
+        <v>0.78639999999999999</v>
+      </c>
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" t="s">
+        <v>50</v>
+      </c>
+      <c r="J23">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>114</v>
+      </c>
+      <c r="M23">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>0.58030000000000004</v>
+      </c>
+      <c r="E24">
+        <v>0.60450000000000004</v>
+      </c>
+      <c r="F24">
+        <v>0.58030000000000004</v>
+      </c>
+      <c r="G24">
+        <v>0.5242</v>
+      </c>
+      <c r="H24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" t="s">
+        <v>50</v>
+      </c>
+      <c r="J24">
+        <v>1.0297000000000001</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>114</v>
+      </c>
+      <c r="M24">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>0.72370000000000001</v>
+      </c>
+      <c r="E25">
+        <v>0.84550000000000003</v>
+      </c>
+      <c r="F25">
+        <v>0.72370000000000001</v>
+      </c>
+      <c r="G25">
+        <v>0.67910000000000004</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25">
+        <v>5.1601999999999997</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" t="s">
+        <v>114</v>
+      </c>
+      <c r="M25">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>0.7409</v>
+      </c>
+      <c r="E26">
+        <v>0.79830000000000001</v>
+      </c>
+      <c r="F26">
+        <v>0.7409</v>
+      </c>
+      <c r="G26">
+        <v>0.74350000000000005</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="K26">
+        <v>1E-4</v>
+      </c>
+      <c r="L26" t="s">
+        <v>114</v>
+      </c>
+      <c r="M26">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="E27">
+        <v>0.54510000000000003</v>
+      </c>
+      <c r="F27">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="G27">
+        <v>0.52629999999999999</v>
+      </c>
+      <c r="H27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27">
+        <v>350</v>
+      </c>
+      <c r="J27">
+        <v>0.87970000000000004</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
+        <v>112</v>
+      </c>
+      <c r="M27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0.51470000000000005</v>
+      </c>
+      <c r="E28">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="F28">
+        <v>0.51470000000000005</v>
+      </c>
+      <c r="G28">
+        <v>0.4461</v>
+      </c>
+      <c r="H28" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28">
+        <v>350</v>
+      </c>
+      <c r="J28">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>112</v>
+      </c>
+      <c r="M28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0.2651</v>
+      </c>
+      <c r="E29">
+        <v>0.214</v>
+      </c>
+      <c r="F29">
+        <v>0.2651</v>
+      </c>
+      <c r="G29">
+        <v>0.20050000000000001</v>
+      </c>
+      <c r="H29" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29">
+        <v>350</v>
+      </c>
+      <c r="J29">
+        <v>1.0572999999999999</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29" t="s">
+        <v>112</v>
+      </c>
+      <c r="M29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.56130000000000002</v>
+      </c>
+      <c r="E30">
+        <v>0.51539999999999997</v>
+      </c>
+      <c r="F30">
+        <v>0.56130000000000002</v>
+      </c>
+      <c r="G30">
+        <v>0.497</v>
+      </c>
+      <c r="H30" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30">
+        <v>350</v>
+      </c>
+      <c r="J30">
+        <v>8.9617000000000004</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30" t="s">
+        <v>112</v>
+      </c>
+      <c r="M30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0.5363</v>
+      </c>
+      <c r="E31">
+        <v>0.50019999999999998</v>
+      </c>
+      <c r="F31">
+        <v>0.5363</v>
+      </c>
+      <c r="G31">
+        <v>0.45419999999999999</v>
+      </c>
+      <c r="H31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31">
+        <v>350</v>
+      </c>
+      <c r="J31">
+        <v>9.5600000000000004E-2</v>
+      </c>
+      <c r="K31">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="L31" t="s">
+        <v>112</v>
+      </c>
+      <c r="M31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M31">
+    <sortCondition descending="1" ref="C2:C31"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>